<commit_message>
added linear regulators + calculations for them, exported parts as library, generated new pdf
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\watchPLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1111C6A5-2280-4511-B9C7-70AC2B3417E0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21A8C94-4E3F-413E-882B-40C2A9CA011D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
   </bookViews>
   <sheets>
     <sheet name="BatteryCharger" sheetId="1" r:id="rId1"/>
     <sheet name="Stromverbrauch" sheetId="2" r:id="rId2"/>
+    <sheet name="Spannungsregler" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>R2</t>
   </si>
@@ -119,6 +120,33 @@
   </si>
   <si>
     <t>BLE</t>
+  </si>
+  <si>
+    <t>4s zu 12.5V</t>
+  </si>
+  <si>
+    <t>Int.referenz</t>
+  </si>
+  <si>
+    <t>4s zu 10V</t>
+  </si>
+  <si>
+    <t>10V zu 3V3</t>
+  </si>
+  <si>
+    <t>R1 (ausgewählt)</t>
+  </si>
+  <si>
+    <t>R2 (Berechnet)</t>
+  </si>
+  <si>
+    <t>R2 (ausgewählt</t>
+  </si>
+  <si>
+    <t>Ausgangsspannung Ziel</t>
+  </si>
+  <si>
+    <t>Ausgangsspannung</t>
   </si>
 </sst>
 </file>
@@ -154,8 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397DA296-EE65-4445-A3C7-1A0E72AFB5DD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -743,4 +772,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3929C5AB-2278-40F5-B04E-501C2C4B16A4}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>1.25</v>
+      </c>
+      <c r="C2">
+        <v>1.25</v>
+      </c>
+      <c r="D2">
+        <v>1.25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>12.5</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>3.3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>5100</v>
+      </c>
+      <c r="C4">
+        <v>5100</v>
+      </c>
+      <c r="D4">
+        <v>5100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <f>((B3/B2)-1)*B4</f>
+        <v>45900</v>
+      </c>
+      <c r="C5">
+        <f>((C3/C2)-1)*C4</f>
+        <v>35700</v>
+      </c>
+      <c r="D5">
+        <f>((D3/D2)-1)*D4</f>
+        <v>8363.9999999999982</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>47000</v>
+      </c>
+      <c r="C6">
+        <v>33000</v>
+      </c>
+      <c r="D6">
+        <v>8200</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1">
+        <f>1.25*(1+(B6/B4))</f>
+        <v>12.769607843137255</v>
+      </c>
+      <c r="C7" s="1">
+        <f>1.25*(1+(C6/C4))</f>
+        <v>9.3382352941176467</v>
+      </c>
+      <c r="D7" s="1">
+        <f>1.25*(1+(D6/D4))</f>
+        <v>3.2598039215686274</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
small schematic changes, started with layout
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\watchPLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21A8C94-4E3F-413E-882B-40C2A9CA011D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8616163-127F-4B8F-81AD-058637459B28}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
   </bookViews>
   <sheets>
     <sheet name="BatteryCharger" sheetId="1" r:id="rId1"/>
     <sheet name="Stromverbrauch" sheetId="2" r:id="rId2"/>
     <sheet name="Spannungsregler" sheetId="3" r:id="rId3"/>
+    <sheet name="Batteriespannungsmessung" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>R2</t>
   </si>
@@ -147,6 +148,24 @@
   </si>
   <si>
     <t>Ausgangsspannung</t>
+  </si>
+  <si>
+    <t>Spannungsteiler</t>
+  </si>
+  <si>
+    <t>Eingang</t>
+  </si>
+  <si>
+    <t>oberer R</t>
+  </si>
+  <si>
+    <t>gewünschte max.Ausgang</t>
+  </si>
+  <si>
+    <t>unterer R</t>
+  </si>
+  <si>
+    <t>berechneter max ausgang</t>
   </si>
 </sst>
 </file>
@@ -778,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3929C5AB-2278-40F5-B04E-501C2C4B16A4}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,4 +931,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3E910B-4AF3-41D0-A293-80A21D887432}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>16.8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>47000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>10000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <f xml:space="preserve"> B3/(B4+B5)*B5</f>
+        <v>2.9473684210526314</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Noticed that I forgot to apply the Calculations for Linear Voltage Regulators to eagle, fixed this
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\watchPLB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8616163-127F-4B8F-81AD-058637459B28}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDC9C3A-02F7-429D-A410-7FD5ED8230DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
   </bookViews>
   <sheets>
     <sheet name="BatteryCharger" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,22 @@
     <sheet name="Spannungsregler" sheetId="3" r:id="rId3"/>
     <sheet name="Batteriespannungsmessung" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>R2</t>
   </si>
@@ -166,6 +171,12 @@
   </si>
   <si>
     <t>berechneter max ausgang</t>
+  </si>
+  <si>
+    <t>R1 unten</t>
+  </si>
+  <si>
+    <t>R2 oben</t>
   </si>
 </sst>
 </file>
@@ -795,10 +806,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3929C5AB-2278-40F5-B04E-501C2C4B16A4}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +820,7 @@
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>31</v>
       </c>
@@ -819,8 +830,11 @@
       <c r="D1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -836,8 +850,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -854,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -871,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -891,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -908,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -937,7 +954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3E910B-4AF3-41D0-A293-80A21D887432}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Accumulated Changes over a few weeks
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\watchPLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EDF2BF-C4DA-4B7E-820F-C39E935E629B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958C3BF7-B469-4BA9-8647-640930542B7D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BDC3154E-11E0-43BD-B7A2-F057E192DB9B}"/>
   </bookViews>
   <sheets>
     <sheet name="BatteryCharger" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Spannungsregler" sheetId="3" r:id="rId3"/>
     <sheet name="Batteriespannungsmessung" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>R2</t>
   </si>
@@ -171,6 +172,15 @@
   </si>
   <si>
     <t>berechneter max ausgang</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>R5 gewählt</t>
+  </si>
+  <si>
+    <t>Vbat error</t>
   </si>
 </sst>
 </file>
@@ -523,18 +533,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3516E887-1242-49EC-8613-3B794B34CA36}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -544,8 +556,15 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1">
+        <f>(0.15*10^-6*E3*B2)/(1.245*(B2+E3))</f>
+        <v>1.3799038518606443E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -559,13 +578,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <f>(B2*(B1-1.245))/(1.245+B2*0.00003)</f>
-        <v>119283.85899814471</v>
+        <f>(B2*(B1-1.245))/(1.245+B2*0.3*10^-6)</f>
+        <v>154463.77090140304</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -573,8 +592,11 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -588,12 +610,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>10000</v>
+        <v>3900</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -602,7 +624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -613,7 +635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -624,24 +646,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.4</v>
+        <v>0.156</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <f>(B7*(B5/B10)-60*10^-6)/B4</f>
+        <v>0.15576000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <f>B5/( (B8*B4)/B7)</f>
-        <v>329999.99999999994</v>
+        <v>330000</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -650,15 +679,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>330000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <f>(B6*B5/B9)/B4</f>
-        <v>3.6363636363636369E-2</v>
-      </c>
-      <c r="C10" t="s">
+        <v>1.4181818181818183E-2</v>
+      </c>
+      <c r="C11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -802,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3929C5AB-2278-40F5-B04E-501C2C4B16A4}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>